<commit_message>
update bom met link naar websites
</commit_message>
<xml_diff>
--- a/documentatie/BOM.xlsx
+++ b/documentatie/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Documents\GitHub\TrappenMaar\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vd_sa\OneDrive\Documenten\KuLeuven\ba3\bachelorproef\TrappenMaar\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD85EFFE-1B4E-4CD5-94B2-28E496B70474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7CD206-6CC6-4094-A07E-5B09759D5A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C76E135C-D577-4759-93DE-929CE909B72A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>BOM</t>
   </si>
@@ -49,21 +49,12 @@
     <t>AANTAL</t>
   </si>
   <si>
-    <t>PRIJS</t>
-  </si>
-  <si>
     <t>reed relay</t>
   </si>
   <si>
     <t>lcd scherm 4x20</t>
   </si>
   <si>
-    <t>double 7 segment display</t>
-  </si>
-  <si>
-    <t>tiny tronics</t>
-  </si>
-  <si>
     <t>snelheidsmeter</t>
   </si>
   <si>
@@ -73,21 +64,9 @@
     <t xml:space="preserve">ledstrip ??? </t>
   </si>
   <si>
-    <t>led diffuser</t>
-  </si>
-  <si>
     <t>Fietsspel</t>
   </si>
   <si>
-    <t>Dik isomo (1 à 2 cm dikte)</t>
-  </si>
-  <si>
-    <t>Dun vel isomo (als diffuser)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> blauwe leds</t>
-  </si>
-  <si>
     <t>groene led</t>
   </si>
   <si>
@@ -97,12 +76,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>rode leds</t>
-  </si>
-  <si>
-    <t>koolweerstanden 220 Ohm</t>
-  </si>
-  <si>
     <t>Weerstand 1kOhm</t>
   </si>
   <si>
@@ -110,6 +83,51 @@
   </si>
   <si>
     <t>Generator Fiets</t>
+  </si>
+  <si>
+    <t>PRIJS/STUK</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/nl/schakelaars/magneetschakelaars/reed-relais-2*14mm</t>
+  </si>
+  <si>
+    <t>ledstrip (domme)</t>
+  </si>
+  <si>
+    <t>dynamo?</t>
+  </si>
+  <si>
+    <t>TOTAAL</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>7 segment display</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/nl/displays/segmenten/segmenten-display-1-karakter-rood</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/nl/componenten/led's/led's/blauwe-led-5mm-diffuus</t>
+  </si>
+  <si>
+    <t>blauwe leds</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/nl/componenten/led's/led's/groene-led-5mm-diffuus</t>
+  </si>
+  <si>
+    <t>3 meter, gaan we statisch houden qua kleur (rood), mogen dus heel simpele leds zijn</t>
+  </si>
+  <si>
+    <t>https://www.action.com/nl-be/p/grundig-multicolor-ledstrip/</t>
+  </si>
+  <si>
+    <t>3 meter liefst individueel adresseerbare leds maar indien dit niet haalbaar is, kunnen we ook werken met de goedkopere variant</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -186,24 +204,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,33 +561,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437F49C8-11C5-45B9-82F1-6E0D7D0F6AFB}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,168 +600,246 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="B7" t="s">
+        <v>24</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E16" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aanmaak BOM 2e bestelronde
</commit_message>
<xml_diff>
--- a/documentatie/BOM.xlsx
+++ b/documentatie/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vd_sa\OneDrive\Documenten\KuLeuven\ba3\bachelorproef\TrappenMaar\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF1B6F-3EBE-40DC-A4ED-920793A3E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848005DB-3260-4C02-9FE6-92950EF0742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C76E135C-D577-4759-93DE-929CE909B72A}"/>
+    <workbookView xWindow="27090" yWindow="3120" windowWidth="57600" windowHeight="15375" xr2:uid="{C76E135C-D577-4759-93DE-929CE909B72A}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -232,6 +232,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,11 +246,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -564,27 +564,27 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="100" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -601,20 +601,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C4">
@@ -627,38 +627,38 @@
         <v>16.440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -666,7 +666,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -683,16 +683,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -745,7 +745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -759,11 +759,11 @@
         <v>0.75</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" ref="E22:E27" si="0">D24*C24</f>
+        <f t="shared" ref="E24:E26" si="0">D24*C24</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -799,7 +799,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -816,16 +816,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -842,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -852,16 +852,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -878,7 +878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -898,29 +898,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{CF3D9E1C-96C5-4A30-8FBD-E0F90BC40BBE}"/>

</xml_diff>